<commit_message>
Changes for the file Path
</commit_message>
<xml_diff>
--- a/src/testData/TestDataSheet.xlsx
+++ b/src/testData/TestDataSheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\orangehrm\src\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4346B973-D3D4-41C4-8257-9452617D9CA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A005065C-D2D8-4292-9977-C13C562FAB02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="73">
   <si>
     <t>Attributes</t>
   </si>
@@ -35,30 +35,12 @@
     <t>Values</t>
   </si>
   <si>
-    <t>screenshotFilePath</t>
-  </si>
-  <si>
-    <t>reportspath</t>
-  </si>
-  <si>
     <t>URL</t>
   </si>
   <si>
     <t>https://opensource-demo.orangehrmlive.com/</t>
   </si>
   <si>
-    <t>intialReport</t>
-  </si>
-  <si>
-    <t>TestDataSheet.xlsx</t>
-  </si>
-  <si>
-    <t>testData</t>
-  </si>
-  <si>
-    <t>testDataFilename</t>
-  </si>
-  <si>
     <t>username</t>
   </si>
   <si>
@@ -98,27 +80,12 @@
     <t>Enabled</t>
   </si>
   <si>
-    <t>E:/workspace/orangehrm/src/libraries/screenshots/</t>
-  </si>
-  <si>
-    <t>E:/workspace/orangehrm/src/libraries/reports/</t>
-  </si>
-  <si>
-    <t>E:/workspace/orangehrm/src/testData/</t>
-  </si>
-  <si>
     <t>Username</t>
   </si>
   <si>
     <t>Password</t>
   </si>
   <si>
-    <t>testdata</t>
-  </si>
-  <si>
-    <t>E:/workspace/orangehrm/src/testData/TestDataSheet.xlsx</t>
-  </si>
-  <si>
     <t>user_role_edit</t>
   </si>
   <si>
@@ -212,9 +179,6 @@
     <t>FKGECEIAMA</t>
   </si>
   <si>
-    <t>E:/workspace/orangehrm/test-output/OrangeHRM-emailable-report-template.html</t>
-  </si>
-  <si>
     <t>FJGFFLCEC</t>
   </si>
   <si>
@@ -240,6 +204,48 @@
   </si>
   <si>
     <t>HNHILGLKGKADCJA</t>
+  </si>
+  <si>
+    <t>BMNCCCKEHKIJEFK</t>
+  </si>
+  <si>
+    <t>tes&amp;2FLM^</t>
+  </si>
+  <si>
+    <t>BMNCCCKEHKIJEFKA</t>
+  </si>
+  <si>
+    <t>ICNJEDHDHLGEKLNLMGFEMBNBGIKEACMBKCMKC</t>
+  </si>
+  <si>
+    <t>&amp;m#ttem6B</t>
+  </si>
+  <si>
+    <t>ICNJEDHDHLGEKLNLMGFEMBNBGIKEACMBKCMKCA</t>
+  </si>
+  <si>
+    <t>DDLJFKLILG</t>
+  </si>
+  <si>
+    <t>7*A %heCA</t>
+  </si>
+  <si>
+    <t>DDLJFKLILGA</t>
+  </si>
+  <si>
+    <t>BCCLMMCIAJ</t>
+  </si>
+  <si>
+    <t>P a9Ae$&amp;a</t>
+  </si>
+  <si>
+    <t>ALJMLIADJFK</t>
+  </si>
+  <si>
+    <t>N@ID8#D1</t>
+  </si>
+  <si>
+    <t>ALJMLIADJFKA</t>
   </si>
 </sst>
 </file>
@@ -578,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -602,61 +608,13 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" xr:uid="{88FCAA25-DC64-449A-8E1B-05A455CF8BD3}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{88FCAA25-DC64-449A-8E1B-05A455CF8BD3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -687,66 +645,66 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -760,7 +718,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF0DF2A2-742A-4463-9C64-15802D677297}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
@@ -769,199 +727,271 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="44.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" t="s">
         <v>60</v>
       </c>
-      <c r="B18" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>62</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B27" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>64</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B28" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="s">
+    <row r="29">
+      <c r="A29" t="s">
         <v>65</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B29" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="s">
+    <row r="30">
+      <c r="A30" t="s">
         <v>67</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B30" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="s">
+    <row r="31">
+      <c r="A31" t="s">
         <v>68</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B31" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="s">
+    <row r="32">
+      <c r="A32" t="s">
         <v>70</v>
       </c>
-      <c r="B24" t="s">
-        <v>70</v>
+      <c r="B32" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>